<commit_message>
set list default select to newest
</commit_message>
<xml_diff>
--- a/SNshare/SNshare.xlsx
+++ b/SNshare/SNshare.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>載入中文=微軟正黑體</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -69,6 +68,16 @@
   <si>
     <t>window color</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>預設選單顯示用distinct event_name和sn_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://mabitool.tk/SNshare/mabi_get.php</t>
+  </si>
+  <si>
+    <t>http://mabitool.ddns.net/SNshare/mabi_get.php</t>
   </si>
 </sst>
 </file>
@@ -418,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:C17"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -525,13 +534,34 @@
         <v>0.54509803921568623</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="1:3">
       <c r="B17">
         <v>175</v>
       </c>
       <c r="C17">
         <f>B17/255</f>
         <v>0.68627450980392157</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
+        <v>43282</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
+        <v>43283</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="B20" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>